<commit_message>
add happy path for ok test case, ignore conditional formatting warning, cleanup after
</commit_message>
<xml_diff>
--- a/tests/data/ok/expected/kozep_proba_osszegzes_input.xlsx
+++ b/tests/data/ok/expected/kozep_proba_osszegzes_input.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Email</t>
   </si>
@@ -28,48 +30,46 @@
     <t>gipszjakab@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Gipsz Jakab</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>gorbe.tamas89@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">Görbe Tamás</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
     <t>kovacsanna@gmail.com</t>
   </si>
   <si>
-    <t>Gipsz Jakab</t>
-  </si>
-  <si>
-    <t>Görbe Tamás</t>
-  </si>
-  <si>
-    <t>Kovacs Anna</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>_</t>
+    <t xml:space="preserve">Kovacs Anna</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="YYYY-MM-DD"/>
   </numFmts>
   <fonts count="2">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -83,11 +83,11 @@
   </fills>
   <borders count="2">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -102,65 +102,35 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDDDDDD"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
@@ -206,13 +176,13 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -240,13 +210,13 @@
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -443,26 +413,243 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="6" width="10.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="23.7109375"/>
+    <col customWidth="1" min="2" max="2" width="11.7109375"/>
+    <col customWidth="1" min="3" max="3" width="5.7109375"/>
+    <col customWidth="1" min="4" max="6" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,29 +669,29 @@
         <v>46006</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -513,44 +700,95 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:F4">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(ROW(),2)=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(),2)=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{002C0053-00E5-4173-9EC7-0064006C0081}">
+            <xm:f>MOD(ROW(),2)=0</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFDDDDDD"/>
+                  <bgColor rgb="FFDDDDDD"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="none"/>
+                <right style="thin">
+                  <color auto="1"/>
+                </right>
+                <top style="none"/>
+                <bottom style="none"/>
+                <diagonal/>
+                <vertical style="none"/>
+                <horizontal style="none"/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A2:F4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="2" id="{000400D1-00A3-4082-A127-00BE00DE00E4}">
+            <xm:f>MOD(ROW(),2)=1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor indexed="65"/>
+                  <bgColor indexed="65"/>
+                </patternFill>
+              </fill>
+              <border>
+                <left style="none"/>
+                <right style="thin">
+                  <color auto="1"/>
+                </right>
+                <top style="none"/>
+                <bottom style="none"/>
+                <diagonal/>
+                <vertical style="none"/>
+                <horizontal style="none"/>
+              </border>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A2:F4</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>